<commit_message>
Purchase Requisition to Post Payment
</commit_message>
<xml_diff>
--- a/templates/POSYDATA.xlsx
+++ b/templates/POSYDATA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dellDevonforce\Provar\ERPFinalProj\rsqasampleproj\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dellDevonforce\Provar\ErpFinalProject\rsqasampleproj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{FB8B842E-64AF-416F-83F9-ED5D944AAF03}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{DBF3E264-27AB-476F-BAC3-D66B28DE898D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="0" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{2D3706E6-F74E-412D-B856-F4DCD436F230}" yWindow="-120"/>
+    <workbookView activeTab="0" firstSheet="6" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{2D3706E6-F74E-412D-B856-F4DCD436F230}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="POReceipt" r:id="rId1" sheetId="1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="46">
   <si>
     <t>Process</t>
   </si>
@@ -159,25 +159,28 @@
     <t>593.0</t>
   </si>
   <si>
-    <t>603.0</t>
-  </si>
-  <si>
     <t>QuantityAfter</t>
   </si>
   <si>
-    <t>613.0</t>
-  </si>
-  <si>
-    <t>780.0</t>
-  </si>
-  <si>
-    <t>790.0</t>
-  </si>
-  <si>
-    <t>948.0</t>
-  </si>
-  <si>
-    <t>958.0</t>
+    <t>970.0</t>
+  </si>
+  <si>
+    <t>980.0</t>
+  </si>
+  <si>
+    <t>a2S1K000001xELw</t>
+  </si>
+  <si>
+    <t>1017.0</t>
+  </si>
+  <si>
+    <t>1027.0</t>
+  </si>
+  <si>
+    <t>1066.0</t>
+  </si>
+  <si>
+    <t>1076.0</t>
   </si>
 </sst>
 </file>
@@ -187,7 +190,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,42 +252,6 @@
       <color indexed="10"/>
       <b val="true"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -294,7 +261,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -314,20 +281,11 @@
     <border>
       <bottom style="thin"/>
     </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0"/>
@@ -336,14 +294,8 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="5" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="7" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="9" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="11" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="12" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="6" fillId="0" fontId="13" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="7" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="4" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -658,9 +610,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C65B3F5-9AF7-4EF8-99A3-B6CFE9D357A8}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
@@ -684,7 +636,7 @@
     <col min="16" max="16" bestFit="true" customWidth="true" width="13.3984375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -731,10 +683,10 @@
         <v>36</v>
       </c>
       <c r="P1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -778,10 +730,10 @@
         <v>34</v>
       </c>
       <c r="O2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="P2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -946,7 +898,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9460007-A700-4ED6-98B4-AD86377C25C9}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,7 +1290,7 @@
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I2">
         <v>4</v>

</xml_diff>